<commit_message>
Sync non localizable files for core commit b490b10c5544defaad50163fa29bfd0c2ca0d902
</commit_message>
<xml_diff>
--- a/help/marketo/product-docs/marketo-sales-insight/actions/getting-started/assets/onboarding-checklist-marketo-sales-insight-actions-2023.xlsx
+++ b/help/marketo/product-docs/marketo-sales-insight/actions/getting-started/assets/onboarding-checklist-marketo-sales-insight-actions-2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewpaul/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adobe-my.sharepoint.com/personal/gluck_adobe_com/Documents/Desktop/GitHub/marketo.en/help/marketo/product-docs/marketo-sales-insight/actions/getting-started/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C029A6-E82E-2F46-8A6F-5080C0A1CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{A6C029A6-E82E-2F46-8A6F-5080C0A1CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D00D1696-101C-47B9-A611-E7CD52146033}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{B53F569E-5990-EB43-AE55-CAD60E181C69}"/>
+    <workbookView xWindow="-21870" yWindow="2205" windowWidth="20340" windowHeight="12780" xr2:uid="{B53F569E-5990-EB43-AE55-CAD60E181C69}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="5" r:id="rId1"/>
@@ -98,12 +98,6 @@
     <t>Actions User</t>
   </si>
   <si>
-    <t>https://experienceleague.corp.adobe.com/docs/marketo/using/product-docs/marketo-sales-insight/actions/phone/call-reasons.html</t>
-  </si>
-  <si>
-    <t>https://experienceleague.corp.adobe.com/docs/marketo/using/product-docs/marketo-sales-insight/actions/phone/call-outcomes.html</t>
-  </si>
-  <si>
     <t>1. Update SFDC Package</t>
   </si>
   <si>
@@ -289,9 +283,6 @@
   <si>
     <t>Ensuring you have the data needed to build reports in Salesforce is important. As an admin, you can configure what infromation related to the activity (e.g., email, call, reminder task) is logged to the subject field in Salesforce so you can better report on your teams' activities in Salesforce. 
 Note: There are dedicated activity fields you can add in Salesforce to log this information to as well, but sometimes you'll want more information in the standard activity subject field in Salesforce.</t>
-  </si>
-  <si>
-    <t>https://experienceleague.adobe.com/docs/marketo/using/product-docs/marketo-sales-connect/crm/salesforce-integration/configure-salesforce-activity-detail-customization.html</t>
   </si>
   <si>
     <t xml:space="preserve">If you use Highspot as a repository for your field and/or sales teams, you can activate the Highspot integration to allow users to grab content from Highspot to add to their emails. </t>
@@ -582,13 +573,22 @@
       <t>Estimated
 5 min</t>
     </r>
+  </si>
+  <si>
+    <t>https://experienceleague.adobe.com/docs/marketo/using/product-docs/marketo-sales-insight/actions/phone/call-reasons.html</t>
+  </si>
+  <si>
+    <t>https://experienceleague.adobe.com/docs/marketo/using/product-docs/marketo-sales-insight/actions/crm/salesforce-integration/configure-salesforce-activity-detail-customization.html</t>
+  </si>
+  <si>
+    <t>https://experienceleague.adobe.com/docs/marketo/using/product-docs/marketo-sales-insight/actions/phone/call-outcomes.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -748,7 +748,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -785,43 +785,34 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1199,23 +1190,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E1ACAA-D9C4-4664-BE72-DE44E77FDD43}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="D27" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="28.375" style="7" customWidth="1"/>
     <col min="4" max="4" width="72.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.625" style="2" customWidth="1"/>
     <col min="6" max="6" width="13" style="2" customWidth="1"/>
     <col min="7" max="7" width="58" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="5"/>
+    <col min="8" max="16384" width="10.875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="11" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1226,566 +1217,555 @@
       <c r="F1" s="10"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="1:7" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:7" s="12" customFormat="1" ht="30" customHeight="1">
+      <c r="A2" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="23.1" customHeight="1">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="102" customHeight="1">
+      <c r="A4" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="122.1" customHeight="1">
+      <c r="A5" s="18"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="138" customHeight="1">
+      <c r="A6" s="18"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="102" customHeight="1">
+      <c r="A7" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="102" customHeight="1">
+      <c r="A8" s="21"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="102" customHeight="1">
+      <c r="A9" s="21"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="102" customHeight="1">
+      <c r="A10" s="21"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="102" customHeight="1">
+      <c r="A11" s="21"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="102" customHeight="1">
+      <c r="A12" s="21"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="D12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="102" customHeight="1">
+      <c r="A13" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="102" customHeight="1">
+      <c r="A14" s="17"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="102" customHeight="1">
+      <c r="A15" s="17"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="102" customHeight="1">
+      <c r="A16" s="17"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="102" customHeight="1">
+      <c r="A17" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="122" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="19" t="s">
+      <c r="C17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="102" customHeight="1">
+      <c r="A18" s="22"/>
+      <c r="C18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="102" customHeight="1">
+      <c r="A19" s="22"/>
+      <c r="C19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="102" customHeight="1">
+      <c r="A20" s="22"/>
+      <c r="C20" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="19" t="s">
+      <c r="F20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="102" customHeight="1">
+      <c r="A21" s="22"/>
+      <c r="C21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="F21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="102" customHeight="1">
+      <c r="A22" s="22"/>
+      <c r="C22" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="102" customHeight="1">
+      <c r="A23" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
+      <c r="C23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="144.94999999999999" customHeight="1">
+      <c r="A24" s="23"/>
+      <c r="C24" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="102" customHeight="1">
+      <c r="A25" s="23"/>
+      <c r="C25" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="102" customHeight="1">
+      <c r="A26" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="19" t="s">
+      <c r="C26" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="19" t="s">
+      <c r="F26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" customFormat="1" ht="102" customHeight="1">
+      <c r="A27" s="17"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18" t="s">
+      <c r="F27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" customFormat="1" ht="102" customHeight="1">
+      <c r="A28" s="17"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="131.1" customHeight="1">
+      <c r="A29" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="19" t="s">
+      <c r="D29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="22"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="19" t="s">
+      <c r="F29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" customFormat="1" ht="102" customHeight="1">
+      <c r="A30" s="18"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="24"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="24"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="145" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="25"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="25"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="22"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="131" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="19" t="s">
+      <c r="F30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="E29" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:7" s="6" customFormat="1">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="7"/>
@@ -1794,7 +1774,7 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" s="6" customFormat="1">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="7"/>
@@ -1803,7 +1783,7 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" s="6" customFormat="1">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="7"/>
@@ -1812,7 +1792,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" s="6" customFormat="1">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="7"/>
@@ -1821,7 +1801,7 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" s="6" customFormat="1">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="7"/>

</xml_diff>

<commit_message>
Sync non localizable files for core commit 1934cbd4a941fdfc1110c6934da66e58042aa572
</commit_message>
<xml_diff>
--- a/help/marketo/product-docs/marketo-sales-insight/actions/getting-started/assets/onboarding-checklist-marketo-sales-insight-actions-2023.xlsx
+++ b/help/marketo/product-docs/marketo-sales-insight/actions/getting-started/assets/onboarding-checklist-marketo-sales-insight-actions-2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adobe-my.sharepoint.com/personal/gluck_adobe_com/Documents/Desktop/GitHub/marketo.en/help/marketo/product-docs/marketo-sales-insight/actions/getting-started/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{A6C029A6-E82E-2F46-8A6F-5080C0A1CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D00D1696-101C-47B9-A611-E7CD52146033}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{A6C029A6-E82E-2F46-8A6F-5080C0A1CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF7D9961-1F38-4B99-8FEC-4124D2252B53}"/>
   <bookViews>
-    <workbookView xWindow="-21870" yWindow="2205" windowWidth="20340" windowHeight="12780" xr2:uid="{B53F569E-5990-EB43-AE55-CAD60E181C69}"/>
+    <workbookView xWindow="30645" yWindow="3015" windowWidth="26880" windowHeight="11295" xr2:uid="{B53F569E-5990-EB43-AE55-CAD60E181C69}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="102">
   <si>
     <t xml:space="preserve">          Marketo Sales Insight Actions | Onboarding Checklist</t>
   </si>
@@ -582,13 +582,16 @@
   </si>
   <si>
     <t>https://experienceleague.adobe.com/docs/marketo/using/product-docs/marketo-sales-insight/actions/phone/call-outcomes.html</t>
+  </si>
+  <si>
+    <t>6. Create Custom Activity Fields in Salesforce</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -665,6 +668,21 @@
       <b/>
       <sz val="30"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -748,7 +766,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -813,6 +831,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -889,6 +916,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1188,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E1ACAA-D9C4-4664-BE72-DE44E77FDD43}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D27" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -1425,34 +1456,33 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="102" customHeight="1">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="21"/>
+      <c r="C13" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="102" customHeight="1">
+      <c r="A14" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="102" customHeight="1">
-      <c r="A14" s="17"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>11</v>
@@ -1461,17 +1491,17 @@
         <v>12</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="102" customHeight="1">
       <c r="A15" s="17"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>11</v>
@@ -1480,17 +1510,17 @@
         <v>12</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="102" customHeight="1">
       <c r="A16" s="17"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>11</v>
@@ -1499,36 +1529,38 @@
         <v>12</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="102" customHeight="1">
-      <c r="A17" s="18" t="s">
-        <v>94</v>
-      </c>
+      <c r="A17" s="17"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="102" customHeight="1">
-      <c r="A18" s="22"/>
+      <c r="A18" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>18</v>
@@ -1537,16 +1569,16 @@
         <v>12</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="102" customHeight="1">
       <c r="A19" s="22"/>
       <c r="C19" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>18</v>
@@ -1555,34 +1587,34 @@
         <v>12</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="102" customHeight="1">
       <c r="A20" s="22"/>
       <c r="C20" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="102" customHeight="1">
       <c r="A21" s="22"/>
       <c r="C21" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>11</v>
@@ -1591,16 +1623,16 @@
         <v>12</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="102" customHeight="1">
       <c r="A22" s="22"/>
       <c r="C22" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>11</v>
@@ -1609,18 +1641,16 @@
         <v>12</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="102" customHeight="1">
-      <c r="A23" s="23" t="s">
-        <v>95</v>
-      </c>
+      <c r="A23" s="22"/>
       <c r="C23" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>11</v>
@@ -1629,16 +1659,18 @@
         <v>12</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="144.94999999999999" customHeight="1">
-      <c r="A24" s="23"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="102" customHeight="1">
+      <c r="A24" s="23" t="s">
+        <v>95</v>
+      </c>
       <c r="C24" s="7" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>11</v>
@@ -1647,55 +1679,54 @@
         <v>12</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="102" customHeight="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="144.94999999999999" customHeight="1">
       <c r="A25" s="23"/>
       <c r="C25" s="7" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="102" customHeight="1">
-      <c r="A26" s="17" t="s">
-        <v>96</v>
-      </c>
+      <c r="A26" s="23"/>
       <c r="C26" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" customFormat="1" ht="102" customHeight="1">
-      <c r="A27" s="17"/>
-      <c r="B27" s="1"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="102" customHeight="1">
+      <c r="A27" s="17" t="s">
+        <v>96</v>
+      </c>
       <c r="C27" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>11</v>
@@ -1703,18 +1734,18 @@
       <c r="F27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="16" t="s">
-        <v>98</v>
+      <c r="G27" s="15" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:7" customFormat="1" ht="102" customHeight="1">
       <c r="A28" s="17"/>
       <c r="B28" s="1"/>
       <c r="C28" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>11</v>
@@ -1723,18 +1754,17 @@
         <v>12</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="131.1" customHeight="1">
-      <c r="A29" s="18" t="s">
-        <v>97</v>
-      </c>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" customFormat="1" ht="102" customHeight="1">
+      <c r="A29" s="17"/>
+      <c r="B29" s="1"/>
       <c r="C29" s="7" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>11</v>
@@ -1742,18 +1772,19 @@
       <c r="F29" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" customFormat="1" ht="102" customHeight="1">
-      <c r="A30" s="18"/>
-      <c r="B30" s="1"/>
+      <c r="G29" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="131.1" customHeight="1">
+      <c r="A30" s="18" t="s">
+        <v>97</v>
+      </c>
       <c r="C30" s="7" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>11</v>
@@ -1761,18 +1792,28 @@
       <c r="F30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="16" t="s">
+      <c r="G30" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" customFormat="1" ht="102" customHeight="1">
+      <c r="A31" s="18"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="16" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" s="6" customFormat="1">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" s="6" customFormat="1">
       <c r="A36" s="1"/>
@@ -1810,16 +1851,25 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
+    <row r="40" spans="1:7" s="6" customFormat="1">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A31"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="A24:A26"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="User Type" prompt="This is the user type that is required to complete this step. " sqref="E3" xr:uid="{BA1D04D6-5AA2-48D5-BF71-1F674D00FDC0}"/>
@@ -1831,35 +1881,36 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="G7" r:id="rId1" xr:uid="{91D5D52B-E592-404E-85AC-90631499880C}"/>
-    <hyperlink ref="G24" r:id="rId2" xr:uid="{B18E8F37-7310-407A-ACFB-EAE7C59450DA}"/>
+    <hyperlink ref="G25" r:id="rId2" xr:uid="{B18E8F37-7310-407A-ACFB-EAE7C59450DA}"/>
     <hyperlink ref="G4" r:id="rId3" xr:uid="{36A38DE5-48FB-432D-9552-5E4B6160C983}"/>
     <hyperlink ref="G5" r:id="rId4" xr:uid="{71CACF5D-906E-4483-B5AC-5431067E2778}"/>
-    <hyperlink ref="G11" r:id="rId5" xr:uid="{5C49CD2D-D653-4199-B65E-5B8BC4ECFBB1}"/>
-    <hyperlink ref="G12" r:id="rId6" xr:uid="{E253D727-1367-455C-86FE-381C9C668123}"/>
-    <hyperlink ref="G13" r:id="rId7" xr:uid="{A06C71ED-34A4-4351-8147-E05035CC24D6}"/>
-    <hyperlink ref="G14" r:id="rId8" xr:uid="{FC836C92-58D0-464A-9A49-D7EC7D8D55DB}"/>
-    <hyperlink ref="G15" r:id="rId9" xr:uid="{05BC4947-F2DE-49DD-9AB8-508D6B961D14}"/>
-    <hyperlink ref="G16" r:id="rId10" xr:uid="{6E367507-BEB6-4BA8-966A-C8D18956CF32}"/>
-    <hyperlink ref="G22" r:id="rId11" xr:uid="{97AB99A9-2267-43C5-8DFF-8F85098DD5A3}"/>
-    <hyperlink ref="G26" r:id="rId12" xr:uid="{BF684940-CBE4-4B35-8A2A-115DAF76FD8F}"/>
-    <hyperlink ref="G8" r:id="rId13" xr:uid="{5BF81A8A-A645-4B49-9348-2F8DC271C86E}"/>
-    <hyperlink ref="G9" r:id="rId14" xr:uid="{F2B98063-B98F-46D8-8C30-F77B12D9A897}"/>
-    <hyperlink ref="G10" r:id="rId15" xr:uid="{9B5E5F5F-0639-4D7A-8908-A7D99A6DB58D}"/>
-    <hyperlink ref="G6" r:id="rId16" xr:uid="{C1E6F230-89C2-4D05-B107-9FAD04E1FC83}"/>
-    <hyperlink ref="G30" r:id="rId17" xr:uid="{4458AE4B-A8B8-40E2-8443-C00720FA13AF}"/>
-    <hyperlink ref="G28" r:id="rId18" xr:uid="{A491AFD2-37AC-4C2B-8029-23FAC49D3E3D}"/>
-    <hyperlink ref="G27" r:id="rId19" xr:uid="{A7B0A59A-A4FD-493C-81A3-0F6ABE0A6FC3}"/>
-    <hyperlink ref="G29" r:id="rId20" xr:uid="{11617860-DD6D-475B-B266-C2AC0DEE045A}"/>
-    <hyperlink ref="G25" r:id="rId21" xr:uid="{31D047E6-D96E-488B-93F3-88D562AB9B6C}"/>
-    <hyperlink ref="G23" r:id="rId22" xr:uid="{43FA1415-6CB3-43D1-9A09-E5DFCAD233CC}"/>
-    <hyperlink ref="G21" r:id="rId23" xr:uid="{6A203741-331F-45D7-A20E-B20FF7C68875}"/>
-    <hyperlink ref="G20" r:id="rId24" xr:uid="{EF748210-3958-40C6-AC73-E9212DD31331}"/>
-    <hyperlink ref="G19" r:id="rId25" xr:uid="{08CF6E90-C420-43B3-8A56-1060D4D84B24}"/>
-    <hyperlink ref="G17" r:id="rId26" xr:uid="{4588488B-AE8B-46E1-919D-9FE07F535C58}"/>
-    <hyperlink ref="G18" r:id="rId27" xr:uid="{2B618DB2-BA9C-428D-BB8B-40A8EE779440}"/>
+    <hyperlink ref="G14" r:id="rId5" xr:uid="{A06C71ED-34A4-4351-8147-E05035CC24D6}"/>
+    <hyperlink ref="G15" r:id="rId6" xr:uid="{FC836C92-58D0-464A-9A49-D7EC7D8D55DB}"/>
+    <hyperlink ref="G16" r:id="rId7" xr:uid="{05BC4947-F2DE-49DD-9AB8-508D6B961D14}"/>
+    <hyperlink ref="G17" r:id="rId8" xr:uid="{6E367507-BEB6-4BA8-966A-C8D18956CF32}"/>
+    <hyperlink ref="G23" r:id="rId9" xr:uid="{97AB99A9-2267-43C5-8DFF-8F85098DD5A3}"/>
+    <hyperlink ref="G27" r:id="rId10" xr:uid="{BF684940-CBE4-4B35-8A2A-115DAF76FD8F}"/>
+    <hyperlink ref="G8" r:id="rId11" xr:uid="{5BF81A8A-A645-4B49-9348-2F8DC271C86E}"/>
+    <hyperlink ref="G9" r:id="rId12" xr:uid="{F2B98063-B98F-46D8-8C30-F77B12D9A897}"/>
+    <hyperlink ref="G10" r:id="rId13" xr:uid="{9B5E5F5F-0639-4D7A-8908-A7D99A6DB58D}"/>
+    <hyperlink ref="G6" r:id="rId14" xr:uid="{C1E6F230-89C2-4D05-B107-9FAD04E1FC83}"/>
+    <hyperlink ref="G31" r:id="rId15" xr:uid="{4458AE4B-A8B8-40E2-8443-C00720FA13AF}"/>
+    <hyperlink ref="G29" r:id="rId16" xr:uid="{A491AFD2-37AC-4C2B-8029-23FAC49D3E3D}"/>
+    <hyperlink ref="G28" r:id="rId17" xr:uid="{A7B0A59A-A4FD-493C-81A3-0F6ABE0A6FC3}"/>
+    <hyperlink ref="G30" r:id="rId18" xr:uid="{11617860-DD6D-475B-B266-C2AC0DEE045A}"/>
+    <hyperlink ref="G26" r:id="rId19" xr:uid="{31D047E6-D96E-488B-93F3-88D562AB9B6C}"/>
+    <hyperlink ref="G24" r:id="rId20" xr:uid="{43FA1415-6CB3-43D1-9A09-E5DFCAD233CC}"/>
+    <hyperlink ref="G22" r:id="rId21" xr:uid="{6A203741-331F-45D7-A20E-B20FF7C68875}"/>
+    <hyperlink ref="G21" r:id="rId22" xr:uid="{EF748210-3958-40C6-AC73-E9212DD31331}"/>
+    <hyperlink ref="G20" r:id="rId23" xr:uid="{08CF6E90-C420-43B3-8A56-1060D4D84B24}"/>
+    <hyperlink ref="G18" r:id="rId24" xr:uid="{4588488B-AE8B-46E1-919D-9FE07F535C58}"/>
+    <hyperlink ref="G19" r:id="rId25" xr:uid="{2B618DB2-BA9C-428D-BB8B-40A8EE779440}"/>
+    <hyperlink ref="G11" r:id="rId26" xr:uid="{FB821474-DB15-4F03-9D1B-752CA0CAFBA4}"/>
+    <hyperlink ref="G12" r:id="rId27" xr:uid="{3F8214E8-79F7-4E4F-BA84-206F75FC14FD}"/>
+    <hyperlink ref="G13" r:id="rId28" display="https://experienceleague.adobe.com/docs/marketo/using/product-docs/marketo-sales-insight/actions/crm/salesforce-configuration/logging-sales-activity-attributes-to-salesforce.html?lang=en" xr:uid="{ECC6F514-19D4-44BD-8FFD-74074C77FC46}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId28"/>
-  <drawing r:id="rId29"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId29"/>
+  <drawing r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>